<commit_message>
Created Sessions dataframe.  This will be used to write the Sessions csv file.
</commit_message>
<xml_diff>
--- a/Sales Enablement - AM EMEA - May 2018.xlsx
+++ b/Sales Enablement - AM EMEA - May 2018.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agruberg/Documents/Data Team/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agruberg/Documents/Data_Team/Sessions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A250064-95B4-084E-93E0-EC11ECA8A06B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8610210A-40CC-4045-9D5C-0AC4F2693715}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="520" windowWidth="24620" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="520" windowWidth="24620" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -3708,8 +3708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G219"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8764,7 +8764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F1932"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>